<commit_message>
1- updating SIQ with developers questions
2- share SIQ with the customer
</commit_message>
<xml_diff>
--- a/SWE/Software Specification/SIQ/SIQ.xlsx
+++ b/SWE/Software Specification/SIQ/SIQ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B893EED-D531-459C-8BFA-A5E039C815A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9A1181-B782-4A49-857F-B06347710490}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Customer Answer</t>
   </si>
   <si>
-    <t>Requirment_Des</t>
-  </si>
-  <si>
     <t>Requirment_IDs</t>
   </si>
   <si>
@@ -43,23 +40,58 @@
   </si>
   <si>
     <t xml:space="preserve">estimated Answer Date </t>
-  </si>
-  <si>
-    <t>ID_HSI or RSC</t>
-  </si>
-  <si>
-    <t>descripe</t>
-  </si>
-  <si>
-    <t>ask</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sovy---Digital-Calculator-PO1_DGC
- SIQ Sheet </t>
   </si>
   <si>
     <t xml:space="preserve">Sovy---Digital-Calculator-PO1_DGC
  SIQ  Sheet </t>
+  </si>
+  <si>
+    <t>PO1_DGCSIQ_1</t>
+  </si>
+  <si>
+    <t>PO1_DGCSIQ_2</t>
+  </si>
+  <si>
+    <t>PO1_DGCSIQ_3</t>
+  </si>
+  <si>
+    <t>PO1_DGCSIQ_4</t>
+  </si>
+  <si>
+    <t>what do you mean by basic mathematical operations ?? do you mean these ?? + - * /</t>
+  </si>
+  <si>
+    <t>how do you want the drawings on the numbers Arabic or English or frensh or chinease ??</t>
+  </si>
+  <si>
+    <t xml:space="preserve">do you want an extra button for power on/off or do you want it included in the keypad ??   
+ if yes do you want a push button or a switch ?? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">do you want a speaker or a buzzer as stated in the HW requiremnets ?? </t>
+  </si>
+  <si>
+    <t>PO1_DGCSIQ_5</t>
+  </si>
+  <si>
+    <t>PO1_DGCSIQ_6</t>
+  </si>
+  <si>
+    <t>PO1_DGCSIQ_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">which tune do you want to play when a btn is pressed ?? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">should the tune be played and ended even if the user is still pressing on the btn ?? 
+ or should it keep playing till he releases the btn ?? </t>
+  </si>
+  <si>
+    <t>how do you want the result shown on the lcd ??
+   do you want it like this 5+5=10 ?? 
+   or like this  __________________
+		|5 + 5 		   |
+		|________________10|</t>
   </si>
 </sst>
 </file>
@@ -181,20 +213,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,113 +525,184 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
-    <col min="6" max="6" width="28.7109375" customWidth="1"/>
+    <col min="1" max="1" width="45.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="18" style="4" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="7">
+        <v>44241</v>
+      </c>
+      <c r="D5" s="7">
+        <v>44241</v>
+      </c>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="B6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="10">
+        <v>44241</v>
+      </c>
+      <c r="D6" s="10">
+        <v>44241</v>
+      </c>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="6">
-        <v>44240</v>
-      </c>
-      <c r="E5" s="6">
-        <v>44242</v>
-      </c>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="B7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="10">
+        <v>44241</v>
+      </c>
+      <c r="D7" s="10">
+        <v>44241</v>
+      </c>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="10">
+        <v>44241</v>
+      </c>
+      <c r="D8" s="10">
+        <v>44241</v>
+      </c>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="10">
+        <v>44241</v>
+      </c>
+      <c r="D9" s="10">
+        <v>44241</v>
+      </c>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="10">
+        <v>44241</v>
+      </c>
+      <c r="D10" s="10">
+        <v>44241</v>
+      </c>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="10">
+        <v>44241</v>
+      </c>
+      <c r="D11" s="10">
+        <v>44241</v>
+      </c>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F3"/>
+    <mergeCell ref="A1:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>